<commit_message>
Mutual Fund and Registration
</commit_message>
<xml_diff>
--- a/HBLAutomationAndroid/Resources/Feature/HBLMobile/Data/BillPayment.xlsx
+++ b/HBLAutomationAndroid/Resources/Feature/HBLMobile/Data/BillPayment.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="64">
   <si>
     <t>Case</t>
   </si>
@@ -99,15 +99,6 @@
     <t>account_no</t>
   </si>
   <si>
-    <t>schedule_type</t>
-  </si>
-  <si>
-    <t>maximum_amount</t>
-  </si>
-  <si>
-    <t>Pay_Transaction_PayBillAmount_RadioBtn</t>
-  </si>
-  <si>
     <t>bene_name</t>
   </si>
   <si>
@@ -144,9 +135,6 @@
     <t>instrument_type</t>
   </si>
   <si>
-    <t>Pay_Transaction_MaxBillAmount_RadioBtn</t>
-  </si>
-  <si>
     <t>account_type</t>
   </si>
   <si>
@@ -163,18 +151,6 @@
   </si>
   <si>
     <t>Abbc</t>
-  </si>
-  <si>
-    <t>Select FIRST_EXECUTION_DATE, LAST_EXECUTION_DATE from DC_SCHEDULED_TRAN_MASTER i where I.CUSTOMER_INFO_ID='{customer_info_id}'</t>
-  </si>
-  <si>
-    <t>Select PARAMTER_VALUE from DC_APPLICATION_PARAM_DETAIL i where I.APPLICATION_PARAMETER_ID='906'</t>
-  </si>
-  <si>
-    <t>schedule_verify</t>
-  </si>
-  <si>
-    <t>schedule_config</t>
   </si>
   <si>
     <t>BillPayment_ConsumerNo_Value</t>
@@ -564,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA10"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,15 +554,12 @@
     <col min="11" max="11" width="185.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16.140625" style="4" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="139.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="118.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="139.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="118.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -603,7 +576,7 @@
         <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>18</v>
@@ -642,10 +615,10 @@
         <v>25</v>
       </c>
       <c r="S1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="T1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="U1" t="s">
         <v>26</v>
@@ -654,45 +627,33 @@
         <v>27</v>
       </c>
       <c r="W1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="X1" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I2">
         <v>12345678</v>
@@ -722,54 +683,45 @@
         <v>20</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="U2" t="s">
-        <v>28</v>
+        <v>42</v>
+      </c>
+      <c r="V2" t="s">
+        <v>39</v>
       </c>
       <c r="W2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="X2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I3">
         <v>12345678</v>
@@ -799,54 +751,42 @@
         <v>20</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="U3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V3" t="s">
+        <v>39</v>
+      </c>
+      <c r="W3" t="s">
         <v>41</v>
       </c>
-      <c r="V3">
-        <v>1000</v>
-      </c>
-      <c r="X3" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA3" t="s">
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" t="s">
-        <v>56</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I4">
         <v>12345678</v>
@@ -876,54 +816,45 @@
         <v>20</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="U4" t="s">
-        <v>28</v>
+        <v>43</v>
+      </c>
+      <c r="V4" t="s">
+        <v>39</v>
       </c>
       <c r="W4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
         <v>47</v>
       </c>
-      <c r="X4" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z4" t="s">
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I5">
         <v>12345678</v>
@@ -953,54 +884,45 @@
         <v>20</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="U5" t="s">
-        <v>28</v>
+        <v>54</v>
+      </c>
+      <c r="V5" t="s">
+        <v>39</v>
       </c>
       <c r="W5" t="s">
-        <v>62</v>
-      </c>
-      <c r="X5" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" t="s">
-        <v>56</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I6">
         <v>12345678</v>
@@ -1030,57 +952,45 @@
         <v>20</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="U6" t="s">
+        <v>55</v>
+      </c>
+      <c r="V6" t="s">
+        <v>39</v>
+      </c>
+      <c r="W6" t="s">
         <v>41</v>
       </c>
-      <c r="V6">
-        <v>1000</v>
-      </c>
-      <c r="W6" t="s">
-        <v>63</v>
-      </c>
-      <c r="X6" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA6" t="s">
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" t="s">
-        <v>56</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I7">
         <v>12345678</v>
@@ -1110,54 +1020,45 @@
         <v>20</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="U7" t="s">
-        <v>28</v>
+        <v>56</v>
+      </c>
+      <c r="V7" t="s">
+        <v>39</v>
       </c>
       <c r="W7" t="s">
-        <v>64</v>
-      </c>
-      <c r="X7" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" t="s">
-        <v>56</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I8">
         <v>12345678</v>
@@ -1187,54 +1088,45 @@
         <v>20</v>
       </c>
       <c r="R8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="U8" t="s">
+        <v>58</v>
+      </c>
+      <c r="V8" t="s">
+        <v>39</v>
+      </c>
+      <c r="W8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="S8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="U8" t="s">
-        <v>28</v>
-      </c>
-      <c r="W8" t="s">
-        <v>66</v>
-      </c>
-      <c r="X8" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I9">
         <v>12345678</v>
@@ -1264,31 +1156,22 @@
         <v>20</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="U9" t="s">
-        <v>28</v>
+        <v>57</v>
+      </c>
+      <c r="V9" t="s">
+        <v>39</v>
       </c>
       <c r="W9" t="s">
-        <v>65</v>
-      </c>
-      <c r="X9" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="3"/>

</xml_diff>